<commit_message>
Handling full pairwise anp model from excel
</commit_message>
<xml_diff>
--- a/examples/anp_data1.xlsx
+++ b/examples/anp_data1.xlsx
@@ -9,7 +9,8 @@
   </bookViews>
   <sheets>
     <sheet name="struct" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="votes" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="connection" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="votes" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="272">
   <si>
     <t xml:space="preserve">Cluster 1</t>
   </si>
@@ -32,49 +33,49 @@
     <t xml:space="preserve">Cluster 3</t>
   </si>
   <si>
-    <t xml:space="preserve">Cluster 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N1-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N3-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N4-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N1-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N3-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N4-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N1-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N3-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N4-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N4-4</t>
+    <t xml:space="preserve">*Cluster 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n1-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n2-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n3-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n4-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n1-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n2-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n3-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n4-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n1-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n2-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n3-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n4-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n2-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n4-4</t>
   </si>
   <si>
     <t xml:space="preserve">User 1</t>
@@ -851,6 +852,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -871,6 +873,7 @@
       <sz val="10"/>
       <name val="Liberation Mono;Courier New;DejaVu Sans Mono;Courier;Monaco"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -944,7 +947,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1032,15 +1035,744 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C253"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C228" activeCellId="0" sqref="C228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.32"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1062,7 +1794,7 @@
       </c>
       <c r="C2" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1071,11 +1803,11 @@
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C3" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,11 +1816,11 @@
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="C4" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1097,7 +1829,7 @@
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
@@ -1110,11 +1842,11 @@
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1123,11 +1855,11 @@
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>0.142857142857143</v>
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,11 +1868,11 @@
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C8" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1149,7 +1881,7 @@
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
@@ -1162,11 +1894,11 @@
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>1</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1175,11 +1907,11 @@
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>0.125</v>
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1188,11 +1920,11 @@
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>5</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1201,11 +1933,11 @@
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1218,7 +1950,7 @@
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1227,11 +1959,11 @@
       </c>
       <c r="B15" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C15" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1240,11 +1972,11 @@
       </c>
       <c r="B16" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C16" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,11 +1985,11 @@
       </c>
       <c r="B17" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1266,11 +1998,11 @@
       </c>
       <c r="B18" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>4</v>
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1279,11 +2011,11 @@
       </c>
       <c r="B19" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>7</v>
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,11 +2024,11 @@
       </c>
       <c r="B20" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C20" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1305,11 +2037,11 @@
       </c>
       <c r="B21" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>4</v>
       </c>
       <c r="C21" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1318,11 +2050,11 @@
       </c>
       <c r="B22" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>5</v>
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1331,11 +2063,11 @@
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>0.25</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1344,11 +2076,11 @@
       </c>
       <c r="B24" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>7</v>
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1361,7 +2093,7 @@
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1370,11 +2102,11 @@
       </c>
       <c r="B26" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>0.125</v>
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1383,11 +2115,11 @@
       </c>
       <c r="B27" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>0.25</v>
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1396,11 +2128,11 @@
       </c>
       <c r="B28" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1409,11 +2141,11 @@
       </c>
       <c r="B29" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1422,11 +2154,11 @@
       </c>
       <c r="B30" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>7</v>
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1435,11 +2167,11 @@
       </c>
       <c r="B31" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1448,11 +2180,11 @@
       </c>
       <c r="B32" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>9</v>
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1461,11 +2193,11 @@
       </c>
       <c r="B33" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>0.111111111111111</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>0.25</v>
-      </c>
-      <c r="C33" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,11 +2206,11 @@
       </c>
       <c r="B34" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1487,11 +2219,11 @@
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1500,11 +2232,11 @@
       </c>
       <c r="B36" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>0.125</v>
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1513,11 +2245,11 @@
       </c>
       <c r="B37" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>2</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>9</v>
-      </c>
-      <c r="C37" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1526,11 +2258,11 @@
       </c>
       <c r="B38" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C38" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1539,11 +2271,11 @@
       </c>
       <c r="B39" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C39" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,11 +2284,11 @@
       </c>
       <c r="B40" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C40" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1565,11 +2297,11 @@
       </c>
       <c r="B41" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C41" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1578,11 +2310,11 @@
       </c>
       <c r="B42" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C42" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1591,11 +2323,11 @@
       </c>
       <c r="B43" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1604,11 +2336,11 @@
       </c>
       <c r="B44" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C44" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1617,11 +2349,11 @@
       </c>
       <c r="B45" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="C45" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1630,11 +2362,11 @@
       </c>
       <c r="B46" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>0.25</v>
       </c>
       <c r="C46" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1643,11 +2375,11 @@
       </c>
       <c r="B47" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="C47" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1656,11 +2388,11 @@
       </c>
       <c r="B48" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C48" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1669,11 +2401,11 @@
       </c>
       <c r="B49" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C49" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1682,11 +2414,11 @@
       </c>
       <c r="B50" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C50" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1695,11 +2427,11 @@
       </c>
       <c r="B51" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.142857142857143</v>
       </c>
       <c r="C51" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1708,11 +2440,11 @@
       </c>
       <c r="B52" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>0.111111111111111</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>3</v>
-      </c>
-      <c r="C52" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1721,11 +2453,11 @@
       </c>
       <c r="B53" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="C53" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,11 +2466,11 @@
       </c>
       <c r="B54" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>0.5</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>0.166666666666667</v>
-      </c>
-      <c r="C54" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1747,11 +2479,11 @@
       </c>
       <c r="B55" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>5</v>
       </c>
       <c r="C55" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1760,7 +2492,7 @@
       </c>
       <c r="B56" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C56" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
@@ -1773,11 +2505,11 @@
       </c>
       <c r="B57" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C57" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1786,11 +2518,11 @@
       </c>
       <c r="B58" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>5</v>
       </c>
       <c r="C58" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1799,11 +2531,11 @@
       </c>
       <c r="B59" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="C59" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1812,11 +2544,11 @@
       </c>
       <c r="B60" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C60" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1825,11 +2557,11 @@
       </c>
       <c r="B61" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="C61" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1838,11 +2570,11 @@
       </c>
       <c r="B62" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="C62" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1851,7 +2583,7 @@
       </c>
       <c r="B63" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="C63" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
@@ -1864,11 +2596,11 @@
       </c>
       <c r="B64" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>9</v>
       </c>
       <c r="C64" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1877,11 +2609,11 @@
       </c>
       <c r="B65" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C65" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1890,11 +2622,11 @@
       </c>
       <c r="B66" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C66" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,11 +2635,11 @@
       </c>
       <c r="B67" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="C67" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1916,11 +2648,11 @@
       </c>
       <c r="B68" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.125</v>
       </c>
       <c r="C68" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1929,11 +2661,11 @@
       </c>
       <c r="B69" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>6</v>
       </c>
       <c r="C69" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1942,11 +2674,11 @@
       </c>
       <c r="B70" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>0.142857142857143</v>
       </c>
       <c r="C70" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1955,11 +2687,11 @@
       </c>
       <c r="B71" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="C71" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1968,11 +2700,11 @@
       </c>
       <c r="B72" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>0.5</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>6</v>
-      </c>
-      <c r="C72" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1981,11 +2713,11 @@
       </c>
       <c r="B73" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C73" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1994,11 +2726,11 @@
       </c>
       <c r="B74" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>0.2</v>
       </c>
       <c r="C74" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2007,11 +2739,11 @@
       </c>
       <c r="B75" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>0.142857142857143</v>
       </c>
       <c r="C75" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2024,7 +2756,7 @@
       </c>
       <c r="C76" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2033,11 +2765,11 @@
       </c>
       <c r="B77" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>1</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>0.25</v>
-      </c>
-      <c r="C77" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2046,11 +2778,11 @@
       </c>
       <c r="B78" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>0.142857142857143</v>
       </c>
       <c r="C78" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2059,11 +2791,11 @@
       </c>
       <c r="B79" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>0.166666666666667</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>0.5</v>
-      </c>
-      <c r="C79" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2072,11 +2804,11 @@
       </c>
       <c r="B80" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="C80" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2085,11 +2817,11 @@
       </c>
       <c r="B81" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C81" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2098,11 +2830,11 @@
       </c>
       <c r="B82" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>9</v>
       </c>
       <c r="C82" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2111,11 +2843,11 @@
       </c>
       <c r="B83" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C83" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2124,11 +2856,11 @@
       </c>
       <c r="B84" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="C84" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2137,7 +2869,7 @@
       </c>
       <c r="B85" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="C85" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
@@ -2150,11 +2882,11 @@
       </c>
       <c r="B86" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C86" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2163,11 +2895,11 @@
       </c>
       <c r="B87" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>1</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>2</v>
-      </c>
-      <c r="C87" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2176,11 +2908,11 @@
       </c>
       <c r="B88" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>0.2</v>
       </c>
       <c r="C88" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2189,11 +2921,11 @@
       </c>
       <c r="B89" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>6</v>
       </c>
       <c r="C89" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2202,11 +2934,11 @@
       </c>
       <c r="B90" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C90" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2215,11 +2947,11 @@
       </c>
       <c r="B91" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C91" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2228,11 +2960,11 @@
       </c>
       <c r="B92" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="C92" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2241,7 +2973,7 @@
       </c>
       <c r="B93" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>4</v>
       </c>
       <c r="C93" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
@@ -2254,7 +2986,7 @@
       </c>
       <c r="B94" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>8</v>
       </c>
       <c r="C94" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
@@ -2267,11 +2999,11 @@
       </c>
       <c r="B95" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>6</v>
       </c>
       <c r="C95" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2280,11 +3012,11 @@
       </c>
       <c r="B96" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C96" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2293,11 +3025,11 @@
       </c>
       <c r="B97" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>0.142857142857143</v>
       </c>
       <c r="C97" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,11 +3038,11 @@
       </c>
       <c r="B98" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>0.2</v>
       </c>
       <c r="C98" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,11 +3051,11 @@
       </c>
       <c r="B99" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C99" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2332,11 +3064,11 @@
       </c>
       <c r="B100" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>0.2</v>
       </c>
       <c r="C100" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2345,11 +3077,11 @@
       </c>
       <c r="B101" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C101" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2358,11 +3090,11 @@
       </c>
       <c r="B102" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C102" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2371,11 +3103,11 @@
       </c>
       <c r="B103" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C103" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2384,11 +3116,11 @@
       </c>
       <c r="B104" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>8</v>
       </c>
       <c r="C104" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2397,11 +3129,11 @@
       </c>
       <c r="B105" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="C105" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2410,11 +3142,11 @@
       </c>
       <c r="B106" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="C106" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2423,11 +3155,11 @@
       </c>
       <c r="B107" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>0.142857142857143</v>
       </c>
       <c r="C107" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2436,11 +3168,11 @@
       </c>
       <c r="B108" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>0.111111111111111</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>3</v>
-      </c>
-      <c r="C108" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2449,11 +3181,11 @@
       </c>
       <c r="B109" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>3</v>
       </c>
       <c r="C109" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2462,11 +3194,11 @@
       </c>
       <c r="B110" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C110" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,11 +3207,11 @@
       </c>
       <c r="B111" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>0.25</v>
       </c>
       <c r="C111" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2488,11 +3220,11 @@
       </c>
       <c r="B112" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>8</v>
       </c>
       <c r="C112" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2501,11 +3233,11 @@
       </c>
       <c r="B113" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>9</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>8</v>
-      </c>
-      <c r="C113" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2514,11 +3246,11 @@
       </c>
       <c r="B114" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.142857142857143</v>
       </c>
       <c r="C114" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2527,11 +3259,11 @@
       </c>
       <c r="B115" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C115" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2544,7 +3276,7 @@
       </c>
       <c r="C116" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2553,11 +3285,11 @@
       </c>
       <c r="B117" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>8</v>
       </c>
       <c r="C117" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2566,11 +3298,11 @@
       </c>
       <c r="B118" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C118" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2579,11 +3311,11 @@
       </c>
       <c r="B119" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C119" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2592,11 +3324,11 @@
       </c>
       <c r="B120" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>0.2</v>
+      </c>
+      <c r="C120" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>0.111111111111111</v>
-      </c>
-      <c r="C120" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2605,11 +3337,11 @@
       </c>
       <c r="B121" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C121" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2618,11 +3350,11 @@
       </c>
       <c r="B122" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>1</v>
+      </c>
+      <c r="C122" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>0.5</v>
-      </c>
-      <c r="C122" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2631,11 +3363,11 @@
       </c>
       <c r="B123" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C123" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2644,11 +3376,11 @@
       </c>
       <c r="B124" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>3</v>
       </c>
       <c r="C124" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2657,11 +3389,11 @@
       </c>
       <c r="B125" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="C125" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2670,11 +3402,11 @@
       </c>
       <c r="B126" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C126" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2683,11 +3415,11 @@
       </c>
       <c r="B127" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C127" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2696,11 +3428,11 @@
       </c>
       <c r="B128" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>8</v>
       </c>
       <c r="C128" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,11 +3441,11 @@
       </c>
       <c r="B129" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="C129" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2722,11 +3454,11 @@
       </c>
       <c r="B130" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C130" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2735,11 +3467,11 @@
       </c>
       <c r="B131" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>0.25</v>
       </c>
       <c r="C131" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2748,11 +3480,11 @@
       </c>
       <c r="B132" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="C132" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2761,11 +3493,11 @@
       </c>
       <c r="B133" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="C133" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2774,11 +3506,11 @@
       </c>
       <c r="B134" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>7</v>
       </c>
       <c r="C134" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2791,7 +3523,7 @@
       </c>
       <c r="C135" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2800,11 +3532,11 @@
       </c>
       <c r="B136" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="C136" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2813,11 +3545,11 @@
       </c>
       <c r="B137" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C137" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2826,7 +3558,7 @@
       </c>
       <c r="B138" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C138" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
@@ -2839,11 +3571,11 @@
       </c>
       <c r="B139" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="C139" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>6</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2852,11 +3584,11 @@
       </c>
       <c r="B140" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C140" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2865,11 +3597,11 @@
       </c>
       <c r="B141" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>0.2</v>
       </c>
       <c r="C141" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2878,11 +3610,11 @@
       </c>
       <c r="B142" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="C142" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2891,11 +3623,11 @@
       </c>
       <c r="B143" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>0.25</v>
       </c>
       <c r="C143" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2904,11 +3636,11 @@
       </c>
       <c r="B144" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>1</v>
       </c>
       <c r="C144" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2917,11 +3649,11 @@
       </c>
       <c r="B145" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C145" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2930,11 +3662,11 @@
       </c>
       <c r="B146" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="C146" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>9</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2943,11 +3675,11 @@
       </c>
       <c r="B147" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>3</v>
       </c>
       <c r="C147" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2956,11 +3688,11 @@
       </c>
       <c r="B148" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C148" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2969,11 +3701,11 @@
       </c>
       <c r="B149" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="C149" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2982,11 +3714,11 @@
       </c>
       <c r="B150" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.125</v>
       </c>
       <c r="C150" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2995,11 +3727,11 @@
       </c>
       <c r="B151" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="C151" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3008,11 +3740,11 @@
       </c>
       <c r="B152" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C152" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3021,11 +3753,11 @@
       </c>
       <c r="B153" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="C153" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3034,11 +3766,11 @@
       </c>
       <c r="B154" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C154" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3051,7 +3783,7 @@
       </c>
       <c r="C155" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>7</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3060,11 +3792,11 @@
       </c>
       <c r="B156" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="C156" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>6</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3073,11 +3805,11 @@
       </c>
       <c r="B157" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C157" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3086,11 +3818,11 @@
       </c>
       <c r="B158" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C158" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3099,11 +3831,11 @@
       </c>
       <c r="B159" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>7</v>
       </c>
       <c r="C159" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3112,11 +3844,11 @@
       </c>
       <c r="B160" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="C160" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3125,11 +3857,11 @@
       </c>
       <c r="B161" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C161" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3138,11 +3870,11 @@
       </c>
       <c r="B162" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C162" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3151,11 +3883,11 @@
       </c>
       <c r="B163" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>0.2</v>
       </c>
       <c r="C163" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3164,11 +3896,11 @@
       </c>
       <c r="B164" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>3</v>
       </c>
       <c r="C164" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3177,11 +3909,11 @@
       </c>
       <c r="B165" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="C165" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3190,11 +3922,11 @@
       </c>
       <c r="B166" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>0.2</v>
       </c>
       <c r="C166" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>9</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3203,11 +3935,11 @@
       </c>
       <c r="B167" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="C167" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>7</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3216,11 +3948,11 @@
       </c>
       <c r="B168" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C168" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3229,11 +3961,11 @@
       </c>
       <c r="B169" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>0.25</v>
+      </c>
+      <c r="C169" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>0.2</v>
-      </c>
-      <c r="C169" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3242,11 +3974,11 @@
       </c>
       <c r="B170" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>4</v>
       </c>
       <c r="C170" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3255,11 +3987,11 @@
       </c>
       <c r="B171" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>6</v>
       </c>
       <c r="C171" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3268,11 +4000,11 @@
       </c>
       <c r="B172" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="C172" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3281,11 +4013,11 @@
       </c>
       <c r="B173" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>0.5</v>
       </c>
       <c r="C173" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3294,11 +4026,11 @@
       </c>
       <c r="B174" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="C174" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>8</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3307,11 +4039,11 @@
       </c>
       <c r="B175" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="C175" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3320,11 +4052,11 @@
       </c>
       <c r="B176" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C176" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3337,7 +4069,7 @@
       </c>
       <c r="C177" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3346,11 +4078,11 @@
       </c>
       <c r="B178" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C178" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3359,11 +4091,11 @@
       </c>
       <c r="B179" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C179" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3372,11 +4104,11 @@
       </c>
       <c r="B180" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C180" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3385,11 +4117,11 @@
       </c>
       <c r="B181" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>6</v>
       </c>
       <c r="C181" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3398,11 +4130,11 @@
       </c>
       <c r="B182" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>0.125</v>
       </c>
       <c r="C182" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3411,11 +4143,11 @@
       </c>
       <c r="B183" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C183" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3424,11 +4156,11 @@
       </c>
       <c r="B184" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="C184" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3437,11 +4169,11 @@
       </c>
       <c r="B185" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C185" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3450,11 +4182,11 @@
       </c>
       <c r="B186" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C186" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3463,11 +4195,11 @@
       </c>
       <c r="B187" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C187" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3476,11 +4208,11 @@
       </c>
       <c r="B188" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C188" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3489,11 +4221,11 @@
       </c>
       <c r="B189" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>4</v>
       </c>
       <c r="C189" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3502,11 +4234,11 @@
       </c>
       <c r="B190" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>0.5</v>
       </c>
       <c r="C190" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3515,11 +4247,11 @@
       </c>
       <c r="B191" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C191" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3528,11 +4260,11 @@
       </c>
       <c r="B192" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>0.2</v>
       </c>
       <c r="C192" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3541,11 +4273,11 @@
       </c>
       <c r="B193" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>3</v>
       </c>
       <c r="C193" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3554,11 +4286,11 @@
       </c>
       <c r="B194" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>0.111111111111111</v>
+      </c>
+      <c r="C194" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>9</v>
-      </c>
-      <c r="C194" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3567,11 +4299,11 @@
       </c>
       <c r="B195" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="C195" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3580,11 +4312,11 @@
       </c>
       <c r="B196" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C196" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>7</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3593,11 +4325,11 @@
       </c>
       <c r="B197" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C197" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3606,11 +4338,11 @@
       </c>
       <c r="B198" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>0.142857142857143</v>
       </c>
       <c r="C198" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>8</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3619,11 +4351,11 @@
       </c>
       <c r="B199" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="C199" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>5</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3632,11 +4364,11 @@
       </c>
       <c r="B200" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C200" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3645,7 +4377,7 @@
       </c>
       <c r="B201" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="C201" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
@@ -3658,11 +4390,11 @@
       </c>
       <c r="B202" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C202" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3671,11 +4403,11 @@
       </c>
       <c r="B203" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>0.25</v>
       </c>
       <c r="C203" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3688,7 +4420,7 @@
       </c>
       <c r="C204" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3697,11 +4429,11 @@
       </c>
       <c r="B205" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C205" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3710,11 +4442,11 @@
       </c>
       <c r="B206" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C206" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3723,11 +4455,11 @@
       </c>
       <c r="B207" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="C207" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3736,11 +4468,11 @@
       </c>
       <c r="B208" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C208" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3749,11 +4481,11 @@
       </c>
       <c r="B209" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>0.142857142857143</v>
       </c>
       <c r="C209" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3762,7 +4494,7 @@
       </c>
       <c r="B210" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C210" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
@@ -3775,11 +4507,11 @@
       </c>
       <c r="B211" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="C211" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3788,7 +4520,7 @@
       </c>
       <c r="B212" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C212" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
@@ -3801,11 +4533,11 @@
       </c>
       <c r="B213" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>0.125</v>
       </c>
       <c r="C213" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3814,11 +4546,11 @@
       </c>
       <c r="B214" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="C214" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3827,11 +4559,11 @@
       </c>
       <c r="B215" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>4</v>
       </c>
       <c r="C215" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3840,11 +4572,11 @@
       </c>
       <c r="B216" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>0.2</v>
       </c>
       <c r="C216" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3853,11 +4585,11 @@
       </c>
       <c r="B217" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>0.2</v>
+      </c>
+      <c r="C217" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>0.142857142857143</v>
-      </c>
-      <c r="C217" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3866,11 +4598,11 @@
       </c>
       <c r="B218" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C218" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3879,11 +4611,11 @@
       </c>
       <c r="B219" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="C219" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3892,11 +4624,11 @@
       </c>
       <c r="B220" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>5</v>
       </c>
       <c r="C220" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3905,11 +4637,11 @@
       </c>
       <c r="B221" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>6</v>
       </c>
       <c r="C221" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3918,11 +4650,11 @@
       </c>
       <c r="B222" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>4</v>
       </c>
       <c r="C222" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3931,11 +4663,11 @@
       </c>
       <c r="B223" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C223" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3944,11 +4676,11 @@
       </c>
       <c r="B224" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="C224" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>6</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3957,11 +4689,11 @@
       </c>
       <c r="B225" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="C225" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3970,11 +4702,11 @@
       </c>
       <c r="B226" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>2</v>
       </c>
       <c r="C226" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3983,11 +4715,11 @@
       </c>
       <c r="B227" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>0.5</v>
       </c>
       <c r="C227" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3996,11 +4728,11 @@
       </c>
       <c r="B228" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C228" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4009,11 +4741,11 @@
       </c>
       <c r="B229" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C229" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4022,11 +4754,11 @@
       </c>
       <c r="B230" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>2</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="C230" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4035,11 +4767,11 @@
       </c>
       <c r="B231" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>9</v>
+      </c>
+      <c r="C231" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>6</v>
-      </c>
-      <c r="C231" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4048,11 +4780,11 @@
       </c>
       <c r="B232" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>0.125</v>
       </c>
       <c r="C232" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4061,11 +4793,11 @@
       </c>
       <c r="B233" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>0.142857142857143</v>
       </c>
       <c r="C233" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4074,11 +4806,11 @@
       </c>
       <c r="B234" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.142857142857143</v>
+        <v>8</v>
       </c>
       <c r="C234" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4087,11 +4819,11 @@
       </c>
       <c r="B235" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="C235" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4100,11 +4832,11 @@
       </c>
       <c r="B236" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C236" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>9</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4113,11 +4845,11 @@
       </c>
       <c r="B237" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>8</v>
       </c>
       <c r="C237" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4126,11 +4858,11 @@
       </c>
       <c r="B238" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>0.2</v>
       </c>
       <c r="C238" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4139,11 +4871,11 @@
       </c>
       <c r="B239" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>4</v>
       </c>
       <c r="C239" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4152,11 +4884,11 @@
       </c>
       <c r="B240" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C240" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4165,11 +4897,11 @@
       </c>
       <c r="B241" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C241" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4178,11 +4910,11 @@
       </c>
       <c r="B242" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C242" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4191,11 +4923,11 @@
       </c>
       <c r="B243" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>9</v>
       </c>
       <c r="C243" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4204,11 +4936,11 @@
       </c>
       <c r="B244" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
+        <v>0.25</v>
       </c>
       <c r="C244" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4217,11 +4949,11 @@
       </c>
       <c r="B245" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C245" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4230,11 +4962,11 @@
       </c>
       <c r="B246" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>6</v>
       </c>
       <c r="C246" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>9</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4243,11 +4975,11 @@
       </c>
       <c r="B247" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="C247" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4256,11 +4988,11 @@
       </c>
       <c r="B248" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>0.111111111111111</v>
       </c>
       <c r="C248" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.166666666666667</v>
+        <v>7</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4269,11 +5001,11 @@
       </c>
       <c r="B249" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
+        <v>0.166666666666667</v>
+      </c>
+      <c r="C249" s="0" t="n">
+        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
         <v>6</v>
-      </c>
-      <c r="C249" s="0" t="n">
-        <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4282,11 +5014,11 @@
       </c>
       <c r="B250" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.5</v>
+        <v>8</v>
       </c>
       <c r="C250" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4295,11 +5027,11 @@
       </c>
       <c r="B251" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C251" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.333333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4308,11 +5040,11 @@
       </c>
       <c r="B252" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C252" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>0.25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4325,13 +5057,13 @@
       </c>
       <c r="C253" s="0" t="n">
         <f aca="false">IF(RANDBETWEEN(0,1)&gt;0, RANDBETWEEN(1,9), 1/RANDBETWEEN(1,9))</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>